<commit_message>
Implemented authentication using regular HTTP Request instead of robot authentication.
</commit_message>
<xml_diff>
--- a/Config/Assets.xlsx
+++ b/Config/Assets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BFC9B1-9563-4ECC-8B77-6325A76848CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F39A2AD-7A7A-422F-B875-BD338D955702}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
   <si>
     <t>Type</t>
   </si>
@@ -109,7 +109,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -166,9 +180,6 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
@@ -211,19 +222,20 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Value"/>
-    <tableColumn id="7" xr3:uid="{9F5282FE-6479-41B7-8672-34D0C5F6C8EE}" name="Folder Id" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{42F54A22-BA7B-4DC3-BF4D-BA0546417160}" name="Id" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{9F5282FE-6479-41B7-8672-34D0C5F6C8EE}" name="Folder Id" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{42F54A22-BA7B-4DC3-BF4D-BA0546417160}" name="Id" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:B101" totalsRowShown="0">
-  <autoFilter ref="A1:B101" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Id" dataDxfId="6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:C101" totalsRowShown="0">
+  <autoFilter ref="A1:C101" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{51051268-0C6E-425F-8AEE-5BD7400426FE}" name="Folder Id" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Id" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -237,8 +249,8 @@
     <tableColumn id="2" xr3:uid="{A5B9750D-9F4C-4ACD-B998-452D86A89786}" name="Type"/>
     <tableColumn id="3" xr3:uid="{C90CC352-910C-44A1-9626-F6DC71398CF0}" name="Description"/>
     <tableColumn id="4" xr3:uid="{FB9ABF1E-6D2B-4148-9C75-B26D470A604D}" name="Value"/>
-    <tableColumn id="7" xr3:uid="{D7BAAF9B-F2D3-47F6-A40B-80DD0288C534}" name="Folder Id" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{C8CEBD6B-CDA3-4576-9A18-16C14163ADBC}" name="Id" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{D7BAAF9B-F2D3-47F6-A40B-80DD0288C534}" name="Folder Id" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{C8CEBD6B-CDA3-4576-9A18-16C14163ADBC}" name="Id" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -253,7 +265,7 @@
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Description"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Value"/>
     <tableColumn id="6" xr3:uid="{C68BBEAC-7A58-41FB-BA92-351982A4DA1B}" name="FolderId" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Id" totalsRowFunction="count" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Id" totalsRowFunction="count" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -994,7 +1006,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A7D921-E601-49D8-BBF5-CB56640085F5}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1003,34 +1015,321 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.36328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="47.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B7" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C43" s="1"/>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C46" s="1"/>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C48" s="1"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C49" s="1"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C50" s="1"/>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C51" s="1"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C52" s="1"/>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C53" s="1"/>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C54" s="1"/>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C55" s="1"/>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C56" s="1"/>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C57" s="1"/>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C58" s="1"/>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C59" s="1"/>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C60" s="1"/>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C61" s="1"/>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C62" s="1"/>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C63" s="1"/>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C64" s="1"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C65" s="1"/>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C66" s="1"/>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C67" s="1"/>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C68" s="1"/>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C69" s="1"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C70" s="1"/>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C71" s="1"/>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C72" s="1"/>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C73" s="1"/>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C74" s="1"/>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C75" s="1"/>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C76" s="1"/>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C77" s="1"/>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C78" s="1"/>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C79" s="1"/>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C80" s="1"/>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C81" s="1"/>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C82" s="1"/>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C83" s="1"/>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C84" s="1"/>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C85" s="1"/>
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C86" s="1"/>
+    </row>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C87" s="1"/>
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C88" s="1"/>
+    </row>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C89" s="1"/>
+    </row>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C90" s="1"/>
+    </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C91" s="1"/>
+    </row>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C92" s="1"/>
+    </row>
+    <row r="93" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C93" s="1"/>
+    </row>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C94" s="1"/>
+    </row>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C95" s="1"/>
+    </row>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C96" s="1"/>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C97" s="1"/>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C98" s="1"/>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C99" s="1"/>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C100" s="1"/>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C101" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implemented writing result of operation to Excel file.
</commit_message>
<xml_diff>
--- a/Config/Assets.xlsx
+++ b/Config/Assets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F39A2AD-7A7A-422F-B875-BD338D955702}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C70C383-0340-4E3F-8D72-B848AA56CFDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
   <si>
     <t>Type</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>FolderId</t>
+  </si>
+  <si>
+    <t>Result</t>
   </si>
 </sst>
 </file>
@@ -109,7 +112,29 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="12">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -123,6 +148,17 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -215,42 +251,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F101" totalsRowShown="0">
-  <autoFilter ref="A1:F101" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G101" totalsRowShown="0">
+  <autoFilter ref="A1:G101" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Value"/>
-    <tableColumn id="7" xr3:uid="{9F5282FE-6479-41B7-8672-34D0C5F6C8EE}" name="Folder Id" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{42F54A22-BA7B-4DC3-BF4D-BA0546417160}" name="Id" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{9F5282FE-6479-41B7-8672-34D0C5F6C8EE}" name="Folder Id" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{42F54A22-BA7B-4DC3-BF4D-BA0546417160}" name="Id" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{E2F843A0-E163-4591-A90A-DA03F637285C}" name="Result" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:C101" totalsRowShown="0">
-  <autoFilter ref="A1:C101" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{51051268-0C6E-425F-8AEE-5BD7400426FE}" name="Folder Id" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Id" dataDxfId="5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:D101" totalsRowShown="0">
+  <autoFilter ref="A1:D101" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{51051268-0C6E-425F-8AEE-5BD7400426FE}" name="Folder Id" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Id" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{789EC9DB-B69B-4343-B58A-CF450EDB59BF}" name="Result" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BD40330C-E043-47F5-9A1D-98C4F5DCAE20}" name="Table15" displayName="Table15" ref="A1:F101" totalsRowShown="0">
-  <autoFilter ref="A1:F101" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BD40330C-E043-47F5-9A1D-98C4F5DCAE20}" name="Table15" displayName="Table15" ref="A1:G101" totalsRowShown="0">
+  <autoFilter ref="A1:G101" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{D002318D-F09E-4941-86F7-CB540B53CA38}" name="Name"/>
     <tableColumn id="2" xr3:uid="{A5B9750D-9F4C-4ACD-B998-452D86A89786}" name="Type"/>
     <tableColumn id="3" xr3:uid="{C90CC352-910C-44A1-9626-F6DC71398CF0}" name="Description"/>
     <tableColumn id="4" xr3:uid="{FB9ABF1E-6D2B-4148-9C75-B26D470A604D}" name="Value"/>
-    <tableColumn id="7" xr3:uid="{D7BAAF9B-F2D3-47F6-A40B-80DD0288C534}" name="Folder Id" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{C8CEBD6B-CDA3-4576-9A18-16C14163ADBC}" name="Id" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{D7BAAF9B-F2D3-47F6-A40B-80DD0288C534}" name="Folder Id" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{C8CEBD6B-CDA3-4576-9A18-16C14163ADBC}" name="Id" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{34576645-A498-4AA2-BA38-3776D490DE1A}" name="Result" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -264,8 +303,8 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Type"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Description"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Value"/>
-    <tableColumn id="6" xr3:uid="{C68BBEAC-7A58-41FB-BA92-351982A4DA1B}" name="FolderId" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Id" totalsRowFunction="count" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{C68BBEAC-7A58-41FB-BA92-351982A4DA1B}" name="FolderId" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Id" totalsRowFunction="count" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -534,7 +573,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -549,7 +588,7 @@
     <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -568,432 +607,538 @@
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
-    </row>
-    <row r="39" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
-    </row>
-    <row r="40" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
-    </row>
-    <row r="41" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
-    </row>
-    <row r="42" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
-    </row>
-    <row r="43" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
-    </row>
-    <row r="44" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
-    </row>
-    <row r="45" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
-    </row>
-    <row r="46" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
-    </row>
-    <row r="47" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
-    </row>
-    <row r="48" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
-    </row>
-    <row r="49" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
-    </row>
-    <row r="50" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
-    </row>
-    <row r="51" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
-    </row>
-    <row r="52" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G51" s="1"/>
+    </row>
+    <row r="52" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
-    </row>
-    <row r="53" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G52" s="1"/>
+    </row>
+    <row r="53" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
-    </row>
-    <row r="54" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G53" s="1"/>
+    </row>
+    <row r="54" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
-    </row>
-    <row r="55" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G54" s="1"/>
+    </row>
+    <row r="55" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
-    </row>
-    <row r="56" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G55" s="1"/>
+    </row>
+    <row r="56" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
-    </row>
-    <row r="57" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G56" s="1"/>
+    </row>
+    <row r="57" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
-    </row>
-    <row r="58" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G57" s="1"/>
+    </row>
+    <row r="58" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
-    </row>
-    <row r="59" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G58" s="1"/>
+    </row>
+    <row r="59" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
-    </row>
-    <row r="60" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G59" s="1"/>
+    </row>
+    <row r="60" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
-    </row>
-    <row r="61" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G60" s="1"/>
+    </row>
+    <row r="61" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
-    </row>
-    <row r="62" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G61" s="1"/>
+    </row>
+    <row r="62" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
-    </row>
-    <row r="63" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G62" s="1"/>
+    </row>
+    <row r="63" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
-    </row>
-    <row r="64" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G63" s="1"/>
+    </row>
+    <row r="64" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
-    </row>
-    <row r="65" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G64" s="1"/>
+    </row>
+    <row r="65" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
-    </row>
-    <row r="66" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G65" s="1"/>
+    </row>
+    <row r="66" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
-    </row>
-    <row r="67" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G66" s="1"/>
+    </row>
+    <row r="67" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
-    </row>
-    <row r="68" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G67" s="1"/>
+    </row>
+    <row r="68" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
-    </row>
-    <row r="69" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G68" s="1"/>
+    </row>
+    <row r="69" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
-    </row>
-    <row r="70" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G69" s="1"/>
+    </row>
+    <row r="70" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
-    </row>
-    <row r="71" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G70" s="1"/>
+    </row>
+    <row r="71" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
-    </row>
-    <row r="72" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G71" s="1"/>
+    </row>
+    <row r="72" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
-    </row>
-    <row r="73" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G72" s="1"/>
+    </row>
+    <row r="73" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
-    </row>
-    <row r="74" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G73" s="1"/>
+    </row>
+    <row r="74" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
-    </row>
-    <row r="75" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G74" s="1"/>
+    </row>
+    <row r="75" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
-    </row>
-    <row r="76" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G75" s="1"/>
+    </row>
+    <row r="76" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
-    </row>
-    <row r="77" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G76" s="1"/>
+    </row>
+    <row r="77" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
-    </row>
-    <row r="78" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G77" s="1"/>
+    </row>
+    <row r="78" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
-    </row>
-    <row r="79" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G78" s="1"/>
+    </row>
+    <row r="79" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
-    </row>
-    <row r="80" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G79" s="1"/>
+    </row>
+    <row r="80" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
-    </row>
-    <row r="81" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G80" s="1"/>
+    </row>
+    <row r="81" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
-    </row>
-    <row r="82" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G81" s="1"/>
+    </row>
+    <row r="82" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
-    </row>
-    <row r="83" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G82" s="1"/>
+    </row>
+    <row r="83" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
-    </row>
-    <row r="84" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G83" s="1"/>
+    </row>
+    <row r="84" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
-    </row>
-    <row r="85" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G84" s="1"/>
+    </row>
+    <row r="85" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
-    </row>
-    <row r="86" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G85" s="1"/>
+    </row>
+    <row r="86" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
-    </row>
-    <row r="87" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G86" s="1"/>
+    </row>
+    <row r="87" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
-    </row>
-    <row r="88" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G87" s="1"/>
+    </row>
+    <row r="88" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
-    </row>
-    <row r="89" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G88" s="1"/>
+    </row>
+    <row r="89" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
-    </row>
-    <row r="90" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G89" s="1"/>
+    </row>
+    <row r="90" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
-    </row>
-    <row r="91" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G90" s="1"/>
+    </row>
+    <row r="91" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
-    </row>
-    <row r="92" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G91" s="1"/>
+    </row>
+    <row r="92" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
-    </row>
-    <row r="93" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G92" s="1"/>
+    </row>
+    <row r="93" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
-    </row>
-    <row r="94" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G93" s="1"/>
+    </row>
+    <row r="94" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
-    </row>
-    <row r="95" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G94" s="1"/>
+    </row>
+    <row r="95" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
-    </row>
-    <row r="96" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G95" s="1"/>
+    </row>
+    <row r="96" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
-    </row>
-    <row r="97" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G96" s="1"/>
+    </row>
+    <row r="97" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
-    </row>
-    <row r="98" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G97" s="1"/>
+    </row>
+    <row r="98" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
-    </row>
-    <row r="99" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G98" s="1"/>
+    </row>
+    <row r="99" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
-    </row>
-    <row r="100" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G99" s="1"/>
+    </row>
+    <row r="100" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
-    </row>
-    <row r="101" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G100" s="1"/>
+    </row>
+    <row r="101" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{F44B3D79-6E85-4752-80E5-E171C2D51A7E}">
       <formula1>"Text,Bool,Integer,Credential"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{0C12A5C3-BDEF-4B44-B330-2C8ED24D0DA9}">
+      <formula1>"Success,Failure"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1006,7 +1151,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A7D921-E601-49D8-BBF5-CB56640085F5}">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1018,7 +1163,7 @@
     <col min="2" max="2" width="13.36328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1028,310 +1173,419 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C30" s="1"/>
-    </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D39" s="1"/>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D41" s="1"/>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C42" s="1"/>
-    </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D42" s="1"/>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C43" s="1"/>
-    </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D43" s="1"/>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C44" s="1"/>
-    </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D44" s="1"/>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C45" s="1"/>
-    </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D45" s="1"/>
+    </row>
+    <row r="46" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C46" s="1"/>
-    </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C47" s="1"/>
-    </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D47" s="1"/>
+    </row>
+    <row r="48" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C48" s="1"/>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D48" s="1"/>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C49" s="1"/>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C50" s="1"/>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D50" s="1"/>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C51" s="1"/>
-    </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D51" s="1"/>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C52" s="1"/>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D52" s="1"/>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C53" s="1"/>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D53" s="1"/>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C54" s="1"/>
-    </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D54" s="1"/>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C55" s="1"/>
-    </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D55" s="1"/>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C56" s="1"/>
-    </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D56" s="1"/>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C57" s="1"/>
-    </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D57" s="1"/>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C58" s="1"/>
-    </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D58" s="1"/>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C59" s="1"/>
-    </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D59" s="1"/>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C60" s="1"/>
-    </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D60" s="1"/>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C61" s="1"/>
-    </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D61" s="1"/>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C62" s="1"/>
-    </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D62" s="1"/>
+    </row>
+    <row r="63" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C63" s="1"/>
-    </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D63" s="1"/>
+    </row>
+    <row r="64" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C64" s="1"/>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D64" s="1"/>
+    </row>
+    <row r="65" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C65" s="1"/>
-    </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D65" s="1"/>
+    </row>
+    <row r="66" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C66" s="1"/>
-    </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D66" s="1"/>
+    </row>
+    <row r="67" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C67" s="1"/>
-    </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D67" s="1"/>
+    </row>
+    <row r="68" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C68" s="1"/>
-    </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D68" s="1"/>
+    </row>
+    <row r="69" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C69" s="1"/>
-    </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D69" s="1"/>
+    </row>
+    <row r="70" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C70" s="1"/>
-    </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D70" s="1"/>
+    </row>
+    <row r="71" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C71" s="1"/>
-    </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D71" s="1"/>
+    </row>
+    <row r="72" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C72" s="1"/>
-    </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D72" s="1"/>
+    </row>
+    <row r="73" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C73" s="1"/>
-    </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D73" s="1"/>
+    </row>
+    <row r="74" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C74" s="1"/>
-    </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D74" s="1"/>
+    </row>
+    <row r="75" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C75" s="1"/>
-    </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D75" s="1"/>
+    </row>
+    <row r="76" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C76" s="1"/>
-    </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D76" s="1"/>
+    </row>
+    <row r="77" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C77" s="1"/>
-    </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D77" s="1"/>
+    </row>
+    <row r="78" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C78" s="1"/>
-    </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D78" s="1"/>
+    </row>
+    <row r="79" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C79" s="1"/>
-    </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D79" s="1"/>
+    </row>
+    <row r="80" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C80" s="1"/>
-    </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D80" s="1"/>
+    </row>
+    <row r="81" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C81" s="1"/>
-    </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D81" s="1"/>
+    </row>
+    <row r="82" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C82" s="1"/>
-    </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D82" s="1"/>
+    </row>
+    <row r="83" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C83" s="1"/>
-    </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D83" s="1"/>
+    </row>
+    <row r="84" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C84" s="1"/>
-    </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D84" s="1"/>
+    </row>
+    <row r="85" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C85" s="1"/>
-    </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D85" s="1"/>
+    </row>
+    <row r="86" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C86" s="1"/>
-    </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D86" s="1"/>
+    </row>
+    <row r="87" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C87" s="1"/>
-    </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D87" s="1"/>
+    </row>
+    <row r="88" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C88" s="1"/>
-    </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D88" s="1"/>
+    </row>
+    <row r="89" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C89" s="1"/>
-    </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D89" s="1"/>
+    </row>
+    <row r="90" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C90" s="1"/>
-    </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D90" s="1"/>
+    </row>
+    <row r="91" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C91" s="1"/>
-    </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D91" s="1"/>
+    </row>
+    <row r="92" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C92" s="1"/>
-    </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D92" s="1"/>
+    </row>
+    <row r="93" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C93" s="1"/>
-    </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D93" s="1"/>
+    </row>
+    <row r="94" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C94" s="1"/>
-    </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D94" s="1"/>
+    </row>
+    <row r="95" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C95" s="1"/>
-    </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D95" s="1"/>
+    </row>
+    <row r="96" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C96" s="1"/>
-    </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D96" s="1"/>
+    </row>
+    <row r="97" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C97" s="1"/>
-    </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D97" s="1"/>
+    </row>
+    <row r="98" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C98" s="1"/>
-    </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D98" s="1"/>
+    </row>
+    <row r="99" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C99" s="1"/>
-    </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D99" s="1"/>
+    </row>
+    <row r="100" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C100" s="1"/>
-    </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D100" s="1"/>
+    </row>
+    <row r="101" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{35099871-3A46-4998-81E8-52CBB353DFB4}">
+      <formula1>"Success,Failure"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -1342,7 +1596,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECF20293-3040-451C-BEA0-1DF5FCF14B01}">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1357,7 +1611,7 @@
     <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1376,431 +1630,537 @@
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
-    </row>
-    <row r="39" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
-    </row>
-    <row r="40" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
-    </row>
-    <row r="41" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
-    </row>
-    <row r="42" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
-    </row>
-    <row r="43" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
-    </row>
-    <row r="44" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
-    </row>
-    <row r="45" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
-    </row>
-    <row r="46" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
-    </row>
-    <row r="47" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
-    </row>
-    <row r="48" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
-    </row>
-    <row r="49" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
-    </row>
-    <row r="50" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
-    </row>
-    <row r="51" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
-    </row>
-    <row r="52" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G51" s="1"/>
+    </row>
+    <row r="52" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
-    </row>
-    <row r="53" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G52" s="1"/>
+    </row>
+    <row r="53" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
-    </row>
-    <row r="54" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G53" s="1"/>
+    </row>
+    <row r="54" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
-    </row>
-    <row r="55" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G54" s="1"/>
+    </row>
+    <row r="55" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
-    </row>
-    <row r="56" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G55" s="1"/>
+    </row>
+    <row r="56" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
-    </row>
-    <row r="57" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G56" s="1"/>
+    </row>
+    <row r="57" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
-    </row>
-    <row r="58" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G57" s="1"/>
+    </row>
+    <row r="58" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
-    </row>
-    <row r="59" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G58" s="1"/>
+    </row>
+    <row r="59" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
-    </row>
-    <row r="60" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G59" s="1"/>
+    </row>
+    <row r="60" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
-    </row>
-    <row r="61" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G60" s="1"/>
+    </row>
+    <row r="61" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
-    </row>
-    <row r="62" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G61" s="1"/>
+    </row>
+    <row r="62" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
-    </row>
-    <row r="63" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G62" s="1"/>
+    </row>
+    <row r="63" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
-    </row>
-    <row r="64" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G63" s="1"/>
+    </row>
+    <row r="64" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
-    </row>
-    <row r="65" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G64" s="1"/>
+    </row>
+    <row r="65" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
-    </row>
-    <row r="66" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G65" s="1"/>
+    </row>
+    <row r="66" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
-    </row>
-    <row r="67" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G66" s="1"/>
+    </row>
+    <row r="67" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
-    </row>
-    <row r="68" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G67" s="1"/>
+    </row>
+    <row r="68" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
-    </row>
-    <row r="69" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G68" s="1"/>
+    </row>
+    <row r="69" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
-    </row>
-    <row r="70" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G69" s="1"/>
+    </row>
+    <row r="70" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
-    </row>
-    <row r="71" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G70" s="1"/>
+    </row>
+    <row r="71" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
-    </row>
-    <row r="72" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G71" s="1"/>
+    </row>
+    <row r="72" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
-    </row>
-    <row r="73" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G72" s="1"/>
+    </row>
+    <row r="73" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
-    </row>
-    <row r="74" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G73" s="1"/>
+    </row>
+    <row r="74" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
-    </row>
-    <row r="75" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G74" s="1"/>
+    </row>
+    <row r="75" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
-    </row>
-    <row r="76" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G75" s="1"/>
+    </row>
+    <row r="76" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
-    </row>
-    <row r="77" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G76" s="1"/>
+    </row>
+    <row r="77" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
-    </row>
-    <row r="78" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G77" s="1"/>
+    </row>
+    <row r="78" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
-    </row>
-    <row r="79" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G78" s="1"/>
+    </row>
+    <row r="79" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
-    </row>
-    <row r="80" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G79" s="1"/>
+    </row>
+    <row r="80" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
-    </row>
-    <row r="81" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G80" s="1"/>
+    </row>
+    <row r="81" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
-    </row>
-    <row r="82" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G81" s="1"/>
+    </row>
+    <row r="82" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
-    </row>
-    <row r="83" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G82" s="1"/>
+    </row>
+    <row r="83" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
-    </row>
-    <row r="84" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G83" s="1"/>
+    </row>
+    <row r="84" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
-    </row>
-    <row r="85" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G84" s="1"/>
+    </row>
+    <row r="85" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
-    </row>
-    <row r="86" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G85" s="1"/>
+    </row>
+    <row r="86" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
-    </row>
-    <row r="87" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G86" s="1"/>
+    </row>
+    <row r="87" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
-    </row>
-    <row r="88" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G87" s="1"/>
+    </row>
+    <row r="88" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
-    </row>
-    <row r="89" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G88" s="1"/>
+    </row>
+    <row r="89" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
-    </row>
-    <row r="90" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G89" s="1"/>
+    </row>
+    <row r="90" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
-    </row>
-    <row r="91" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G90" s="1"/>
+    </row>
+    <row r="91" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
-    </row>
-    <row r="92" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G91" s="1"/>
+    </row>
+    <row r="92" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
-    </row>
-    <row r="93" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G92" s="1"/>
+    </row>
+    <row r="93" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
-    </row>
-    <row r="94" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G93" s="1"/>
+    </row>
+    <row r="94" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
-    </row>
-    <row r="95" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G94" s="1"/>
+    </row>
+    <row r="95" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
-    </row>
-    <row r="96" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G95" s="1"/>
+    </row>
+    <row r="96" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
-    </row>
-    <row r="97" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G96" s="1"/>
+    </row>
+    <row r="97" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
-    </row>
-    <row r="98" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G97" s="1"/>
+    </row>
+    <row r="98" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
-    </row>
-    <row r="99" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G98" s="1"/>
+    </row>
+    <row r="99" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
-    </row>
-    <row r="100" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G99" s="1"/>
+    </row>
+    <row r="100" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
-    </row>
-    <row r="101" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="G100" s="1"/>
+    </row>
+    <row r="101" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{63D27801-1665-4DF8-9454-ACFF98F813D0}">
       <formula1>"Text,Bool,Integer,Credential"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{058D4C25-5E40-4180-A841-99A1B244C3D1}">
+      <formula1>"Success,Failure"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implemented getting assets from all folders or from a specified folder.
</commit_message>
<xml_diff>
--- a/Config/Assets.xlsx
+++ b/Config/Assets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C70C383-0340-4E3F-8D72-B848AA56CFDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897E8C4A-41FF-40C4-9A1C-4AF6F0764907}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="9">
   <si>
     <t>Type</t>
   </si>
@@ -56,10 +56,13 @@
     <t>Folder Id</t>
   </si>
   <si>
-    <t>FolderId</t>
+    <t>Result</t>
   </si>
   <si>
-    <t>Result</t>
+    <t>Folder Name</t>
+  </si>
+  <si>
+    <t>Asset Id</t>
   </si>
 </sst>
 </file>
@@ -112,7 +115,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="15">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -145,9 +168,6 @@
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -258,9 +278,9 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Value"/>
-    <tableColumn id="7" xr3:uid="{9F5282FE-6479-41B7-8672-34D0C5F6C8EE}" name="Folder Id" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{42F54A22-BA7B-4DC3-BF4D-BA0546417160}" name="Id" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{E2F843A0-E163-4591-A90A-DA03F637285C}" name="Result" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{9F5282FE-6479-41B7-8672-34D0C5F6C8EE}" name="Folder Id" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{42F54A22-BA7B-4DC3-BF4D-BA0546417160}" name="Id" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{E2F843A0-E163-4591-A90A-DA03F637285C}" name="Result" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -270,10 +290,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:D101" totalsRowShown="0">
   <autoFilter ref="A1:D101" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{51051268-0C6E-425F-8AEE-5BD7400426FE}" name="Folder Id" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Id" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{789EC9DB-B69B-4343-B58A-CF450EDB59BF}" name="Result" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{51051268-0C6E-425F-8AEE-5BD7400426FE}" name="Folder Id" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Id" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{789EC9DB-B69B-4343-B58A-CF450EDB59BF}" name="Result" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -287,24 +307,25 @@
     <tableColumn id="2" xr3:uid="{A5B9750D-9F4C-4ACD-B998-452D86A89786}" name="Type"/>
     <tableColumn id="3" xr3:uid="{C90CC352-910C-44A1-9626-F6DC71398CF0}" name="Description"/>
     <tableColumn id="4" xr3:uid="{FB9ABF1E-6D2B-4148-9C75-B26D470A604D}" name="Value"/>
-    <tableColumn id="7" xr3:uid="{D7BAAF9B-F2D3-47F6-A40B-80DD0288C534}" name="Folder Id" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{C8CEBD6B-CDA3-4576-9A18-16C14163ADBC}" name="Id" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{34576645-A498-4AA2-BA38-3776D490DE1A}" name="Result" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{D7BAAF9B-F2D3-47F6-A40B-80DD0288C534}" name="Folder Id" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{C8CEBD6B-CDA3-4576-9A18-16C14163ADBC}" name="Id" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{34576645-A498-4AA2-BA38-3776D490DE1A}" name="Result" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:F101">
-  <autoFilter ref="A1:F101" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:G101">
+  <autoFilter ref="A1:G101" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Type"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Description"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Value"/>
-    <tableColumn id="6" xr3:uid="{C68BBEAC-7A58-41FB-BA92-351982A4DA1B}" name="FolderId" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Id" totalsRowFunction="count" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Description" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Value" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{A067D188-197D-4A79-82E6-8C9B8EDABB7C}" name="Asset Id" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{C68BBEAC-7A58-41FB-BA92-351982A4DA1B}" name="Folder Name" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Folder Id" totalsRowFunction="count" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -575,7 +596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -608,7 +629,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -1174,7 +1195,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -1631,7 +1652,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -2173,9 +2194,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B90804-4CC2-4F3A-A5A0-B313E9BACDDF}">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2183,12 +2204,14 @@
   <cols>
     <col min="1" max="1" width="13" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.36328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="48.81640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="47.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.81640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="38.6328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" customWidth="1"/>
+    <col min="6" max="6" width="16.1796875" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2202,429 +2225,514 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E15" s="1"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F15" s="1"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E16" s="1"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F16" s="1"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E17" s="1"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F17" s="1"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E18" s="1"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F18" s="1"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E19" s="1"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F19" s="1"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E20" s="1"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F20" s="1"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E21" s="1"/>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F21" s="1"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E22" s="1"/>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F22" s="1"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E23" s="1"/>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F23" s="1"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E24" s="1"/>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F24" s="1"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E25" s="1"/>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F25" s="1"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E26" s="1"/>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F26" s="1"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E27" s="1"/>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F27" s="1"/>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E28" s="1"/>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F28" s="1"/>
+      <c r="G28" s="3"/>
+    </row>
+    <row r="29" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E29" s="1"/>
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F29" s="1"/>
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E30" s="1"/>
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F30" s="1"/>
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E31" s="1"/>
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F31" s="1"/>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E32" s="1"/>
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F32" s="1"/>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E33" s="1"/>
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F33" s="1"/>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E34" s="1"/>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F34" s="1"/>
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E35" s="1"/>
-      <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F35" s="1"/>
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E36" s="1"/>
-      <c r="F36" s="3"/>
-    </row>
-    <row r="37" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F36" s="1"/>
+      <c r="G36" s="3"/>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E37" s="1"/>
-      <c r="F37" s="3"/>
-    </row>
-    <row r="38" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F37" s="1"/>
+      <c r="G37" s="3"/>
+    </row>
+    <row r="38" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E38" s="1"/>
-      <c r="F38" s="3"/>
-    </row>
-    <row r="39" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F38" s="1"/>
+      <c r="G38" s="3"/>
+    </row>
+    <row r="39" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E39" s="1"/>
-      <c r="F39" s="3"/>
-    </row>
-    <row r="40" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F39" s="1"/>
+      <c r="G39" s="3"/>
+    </row>
+    <row r="40" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E40" s="1"/>
-      <c r="F40" s="3"/>
-    </row>
-    <row r="41" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F40" s="1"/>
+      <c r="G40" s="3"/>
+    </row>
+    <row r="41" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E41" s="1"/>
-      <c r="F41" s="3"/>
-    </row>
-    <row r="42" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F41" s="1"/>
+      <c r="G41" s="3"/>
+    </row>
+    <row r="42" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E42" s="1"/>
-      <c r="F42" s="3"/>
-    </row>
-    <row r="43" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F42" s="1"/>
+      <c r="G42" s="3"/>
+    </row>
+    <row r="43" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E43" s="1"/>
-      <c r="F43" s="3"/>
-    </row>
-    <row r="44" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F43" s="1"/>
+      <c r="G43" s="3"/>
+    </row>
+    <row r="44" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E44" s="1"/>
-      <c r="F44" s="3"/>
-    </row>
-    <row r="45" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F44" s="1"/>
+      <c r="G44" s="3"/>
+    </row>
+    <row r="45" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E45" s="1"/>
-      <c r="F45" s="3"/>
-    </row>
-    <row r="46" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F45" s="1"/>
+      <c r="G45" s="3"/>
+    </row>
+    <row r="46" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E46" s="1"/>
-      <c r="F46" s="3"/>
-    </row>
-    <row r="47" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F46" s="1"/>
+      <c r="G46" s="3"/>
+    </row>
+    <row r="47" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E47" s="1"/>
-      <c r="F47" s="3"/>
-    </row>
-    <row r="48" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F47" s="1"/>
+      <c r="G47" s="3"/>
+    </row>
+    <row r="48" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E48" s="1"/>
-      <c r="F48" s="3"/>
-    </row>
-    <row r="49" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F48" s="1"/>
+      <c r="G48" s="3"/>
+    </row>
+    <row r="49" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E49" s="1"/>
-      <c r="F49" s="3"/>
-    </row>
-    <row r="50" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F49" s="1"/>
+      <c r="G49" s="3"/>
+    </row>
+    <row r="50" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E50" s="1"/>
-      <c r="F50" s="3"/>
-    </row>
-    <row r="51" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F50" s="1"/>
+      <c r="G50" s="3"/>
+    </row>
+    <row r="51" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E51" s="1"/>
-      <c r="F51" s="3"/>
-    </row>
-    <row r="52" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F51" s="1"/>
+      <c r="G51" s="3"/>
+    </row>
+    <row r="52" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E52" s="1"/>
-      <c r="F52" s="3"/>
-    </row>
-    <row r="53" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F52" s="1"/>
+      <c r="G52" s="3"/>
+    </row>
+    <row r="53" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E53" s="1"/>
-      <c r="F53" s="3"/>
-    </row>
-    <row r="54" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F53" s="1"/>
+      <c r="G53" s="3"/>
+    </row>
+    <row r="54" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E54" s="1"/>
-      <c r="F54" s="3"/>
-    </row>
-    <row r="55" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F54" s="1"/>
+      <c r="G54" s="3"/>
+    </row>
+    <row r="55" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E55" s="1"/>
-      <c r="F55" s="3"/>
-    </row>
-    <row r="56" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F55" s="1"/>
+      <c r="G55" s="3"/>
+    </row>
+    <row r="56" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E56" s="1"/>
-      <c r="F56" s="3"/>
-    </row>
-    <row r="57" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F56" s="1"/>
+      <c r="G56" s="3"/>
+    </row>
+    <row r="57" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E57" s="1"/>
-      <c r="F57" s="3"/>
-    </row>
-    <row r="58" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F57" s="1"/>
+      <c r="G57" s="3"/>
+    </row>
+    <row r="58" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E58" s="1"/>
-      <c r="F58" s="3"/>
-    </row>
-    <row r="59" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F58" s="1"/>
+      <c r="G58" s="3"/>
+    </row>
+    <row r="59" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E59" s="1"/>
-      <c r="F59" s="3"/>
-    </row>
-    <row r="60" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F59" s="1"/>
+      <c r="G59" s="3"/>
+    </row>
+    <row r="60" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E60" s="1"/>
-      <c r="F60" s="3"/>
-    </row>
-    <row r="61" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F60" s="1"/>
+      <c r="G60" s="3"/>
+    </row>
+    <row r="61" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E61" s="1"/>
-      <c r="F61" s="3"/>
-    </row>
-    <row r="62" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F61" s="1"/>
+      <c r="G61" s="3"/>
+    </row>
+    <row r="62" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E62" s="1"/>
-      <c r="F62" s="3"/>
-    </row>
-    <row r="63" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F62" s="1"/>
+      <c r="G62" s="3"/>
+    </row>
+    <row r="63" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E63" s="1"/>
-      <c r="F63" s="3"/>
-    </row>
-    <row r="64" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F63" s="1"/>
+      <c r="G63" s="3"/>
+    </row>
+    <row r="64" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E64" s="1"/>
-      <c r="F64" s="3"/>
-    </row>
-    <row r="65" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F64" s="1"/>
+      <c r="G64" s="3"/>
+    </row>
+    <row r="65" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E65" s="1"/>
-      <c r="F65" s="3"/>
-    </row>
-    <row r="66" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F65" s="1"/>
+      <c r="G65" s="3"/>
+    </row>
+    <row r="66" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E66" s="1"/>
-      <c r="F66" s="3"/>
-    </row>
-    <row r="67" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F66" s="1"/>
+      <c r="G66" s="3"/>
+    </row>
+    <row r="67" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E67" s="1"/>
-      <c r="F67" s="3"/>
-    </row>
-    <row r="68" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F67" s="1"/>
+      <c r="G67" s="3"/>
+    </row>
+    <row r="68" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E68" s="1"/>
-      <c r="F68" s="3"/>
-    </row>
-    <row r="69" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F68" s="1"/>
+      <c r="G68" s="3"/>
+    </row>
+    <row r="69" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E69" s="1"/>
-      <c r="F69" s="3"/>
-    </row>
-    <row r="70" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F69" s="1"/>
+      <c r="G69" s="3"/>
+    </row>
+    <row r="70" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E70" s="1"/>
-      <c r="F70" s="3"/>
-    </row>
-    <row r="71" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F70" s="1"/>
+      <c r="G70" s="3"/>
+    </row>
+    <row r="71" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E71" s="1"/>
-      <c r="F71" s="3"/>
-    </row>
-    <row r="72" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F71" s="1"/>
+      <c r="G71" s="3"/>
+    </row>
+    <row r="72" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E72" s="1"/>
-      <c r="F72" s="3"/>
-    </row>
-    <row r="73" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F72" s="1"/>
+      <c r="G72" s="3"/>
+    </row>
+    <row r="73" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E73" s="1"/>
-      <c r="F73" s="3"/>
-    </row>
-    <row r="74" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F73" s="1"/>
+      <c r="G73" s="3"/>
+    </row>
+    <row r="74" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E74" s="1"/>
-      <c r="F74" s="3"/>
-    </row>
-    <row r="75" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F74" s="1"/>
+      <c r="G74" s="3"/>
+    </row>
+    <row r="75" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E75" s="1"/>
-      <c r="F75" s="3"/>
-    </row>
-    <row r="76" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F75" s="1"/>
+      <c r="G75" s="3"/>
+    </row>
+    <row r="76" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E76" s="1"/>
-      <c r="F76" s="3"/>
-    </row>
-    <row r="77" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F76" s="1"/>
+      <c r="G76" s="3"/>
+    </row>
+    <row r="77" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E77" s="1"/>
-      <c r="F77" s="3"/>
-    </row>
-    <row r="78" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F77" s="1"/>
+      <c r="G77" s="3"/>
+    </row>
+    <row r="78" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E78" s="1"/>
-      <c r="F78" s="3"/>
-    </row>
-    <row r="79" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F78" s="1"/>
+      <c r="G78" s="3"/>
+    </row>
+    <row r="79" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E79" s="1"/>
-      <c r="F79" s="3"/>
-    </row>
-    <row r="80" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F79" s="1"/>
+      <c r="G79" s="3"/>
+    </row>
+    <row r="80" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E80" s="1"/>
-      <c r="F80" s="3"/>
-    </row>
-    <row r="81" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F80" s="1"/>
+      <c r="G80" s="3"/>
+    </row>
+    <row r="81" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E81" s="1"/>
-      <c r="F81" s="3"/>
-    </row>
-    <row r="82" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F81" s="1"/>
+      <c r="G81" s="3"/>
+    </row>
+    <row r="82" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E82" s="1"/>
-      <c r="F82" s="3"/>
-    </row>
-    <row r="83" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F82" s="1"/>
+      <c r="G82" s="3"/>
+    </row>
+    <row r="83" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E83" s="1"/>
-      <c r="F83" s="3"/>
-    </row>
-    <row r="84" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F83" s="1"/>
+      <c r="G83" s="3"/>
+    </row>
+    <row r="84" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E84" s="1"/>
-      <c r="F84" s="3"/>
-    </row>
-    <row r="85" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F84" s="1"/>
+      <c r="G84" s="3"/>
+    </row>
+    <row r="85" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E85" s="1"/>
-      <c r="F85" s="3"/>
-    </row>
-    <row r="86" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F85" s="1"/>
+      <c r="G85" s="3"/>
+    </row>
+    <row r="86" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E86" s="1"/>
-      <c r="F86" s="3"/>
-    </row>
-    <row r="87" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F86" s="1"/>
+      <c r="G86" s="3"/>
+    </row>
+    <row r="87" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E87" s="1"/>
-      <c r="F87" s="3"/>
-    </row>
-    <row r="88" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F87" s="1"/>
+      <c r="G87" s="3"/>
+    </row>
+    <row r="88" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E88" s="1"/>
-      <c r="F88" s="3"/>
-    </row>
-    <row r="89" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F88" s="1"/>
+      <c r="G88" s="3"/>
+    </row>
+    <row r="89" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E89" s="1"/>
-      <c r="F89" s="3"/>
-    </row>
-    <row r="90" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F89" s="1"/>
+      <c r="G89" s="3"/>
+    </row>
+    <row r="90" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E90" s="1"/>
-      <c r="F90" s="3"/>
-    </row>
-    <row r="91" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F90" s="1"/>
+      <c r="G90" s="3"/>
+    </row>
+    <row r="91" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E91" s="1"/>
-      <c r="F91" s="3"/>
-    </row>
-    <row r="92" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F91" s="1"/>
+      <c r="G91" s="3"/>
+    </row>
+    <row r="92" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E92" s="1"/>
-      <c r="F92" s="3"/>
-    </row>
-    <row r="93" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F92" s="1"/>
+      <c r="G92" s="3"/>
+    </row>
+    <row r="93" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E93" s="1"/>
-      <c r="F93" s="3"/>
-    </row>
-    <row r="94" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F93" s="1"/>
+      <c r="G93" s="3"/>
+    </row>
+    <row r="94" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E94" s="1"/>
-      <c r="F94" s="3"/>
-    </row>
-    <row r="95" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F94" s="1"/>
+      <c r="G94" s="3"/>
+    </row>
+    <row r="95" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E95" s="1"/>
-      <c r="F95" s="3"/>
-    </row>
-    <row r="96" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F95" s="1"/>
+      <c r="G95" s="3"/>
+    </row>
+    <row r="96" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E96" s="1"/>
-      <c r="F96" s="3"/>
-    </row>
-    <row r="97" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F96" s="1"/>
+      <c r="G96" s="3"/>
+    </row>
+    <row r="97" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E97" s="1"/>
-      <c r="F97" s="3"/>
-    </row>
-    <row r="98" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F97" s="1"/>
+      <c r="G97" s="3"/>
+    </row>
+    <row r="98" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E98" s="1"/>
-      <c r="F98" s="3"/>
-    </row>
-    <row r="99" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F98" s="1"/>
+      <c r="G98" s="3"/>
+    </row>
+    <row r="99" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E99" s="1"/>
-      <c r="F99" s="3"/>
-    </row>
-    <row r="100" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F99" s="1"/>
+      <c r="G99" s="3"/>
+    </row>
+    <row r="100" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E100" s="1"/>
-      <c r="F100" s="3"/>
-    </row>
-    <row r="101" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F100" s="1"/>
+      <c r="G100" s="3"/>
+    </row>
+    <row r="101" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E101" s="1"/>
-      <c r="F101" s="3"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Creation of assets now accept folder path in addition to folder Id.
</commit_message>
<xml_diff>
--- a/Config/Assets.xlsx
+++ b/Config/Assets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897E8C4A-41FF-40C4-9A1C-4AF6F0764907}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B51AF56-9024-4A02-98CA-675E92F14E63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create" sheetId="1" r:id="rId1"/>
@@ -47,9 +47,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Id</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -63,6 +60,9 @@
   </si>
   <si>
     <t>Asset Id</t>
+  </si>
+  <si>
+    <t>Folder Id or Path</t>
   </si>
 </sst>
 </file>
@@ -117,26 +117,6 @@
   </cellStyles>
   <dxfs count="15">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
@@ -170,6 +150,9 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
@@ -179,6 +162,23 @@
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -278,9 +278,9 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Value"/>
-    <tableColumn id="7" xr3:uid="{9F5282FE-6479-41B7-8672-34D0C5F6C8EE}" name="Folder Id" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{42F54A22-BA7B-4DC3-BF4D-BA0546417160}" name="Id" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{E2F843A0-E163-4591-A90A-DA03F637285C}" name="Result" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{9F5282FE-6479-41B7-8672-34D0C5F6C8EE}" name="Folder Id or Path" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{42F54A22-BA7B-4DC3-BF4D-BA0546417160}" name="Asset Id" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{E2F843A0-E163-4591-A90A-DA03F637285C}" name="Result" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -290,10 +290,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:D101" totalsRowShown="0">
   <autoFilter ref="A1:D101" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{51051268-0C6E-425F-8AEE-5BD7400426FE}" name="Folder Id" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Id" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{789EC9DB-B69B-4343-B58A-CF450EDB59BF}" name="Result" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{51051268-0C6E-425F-8AEE-5BD7400426FE}" name="Folder Id or Path" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Asset Id" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{789EC9DB-B69B-4343-B58A-CF450EDB59BF}" name="Result" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -307,9 +307,9 @@
     <tableColumn id="2" xr3:uid="{A5B9750D-9F4C-4ACD-B998-452D86A89786}" name="Type"/>
     <tableColumn id="3" xr3:uid="{C90CC352-910C-44A1-9626-F6DC71398CF0}" name="Description"/>
     <tableColumn id="4" xr3:uid="{FB9ABF1E-6D2B-4148-9C75-B26D470A604D}" name="Value"/>
-    <tableColumn id="7" xr3:uid="{D7BAAF9B-F2D3-47F6-A40B-80DD0288C534}" name="Folder Id" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{C8CEBD6B-CDA3-4576-9A18-16C14163ADBC}" name="Id" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{34576645-A498-4AA2-BA38-3776D490DE1A}" name="Result" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{D7BAAF9B-F2D3-47F6-A40B-80DD0288C534}" name="Folder Id or Path" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{C8CEBD6B-CDA3-4576-9A18-16C14163ADBC}" name="Asset Id" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{34576645-A498-4AA2-BA38-3776D490DE1A}" name="Result" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -321,9 +321,9 @@
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Type"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Description" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Value" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{A067D188-197D-4A79-82E6-8C9B8EDABB7C}" name="Asset Id" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Description" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Value" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{A067D188-197D-4A79-82E6-8C9B8EDABB7C}" name="Asset Id" dataDxfId="5"/>
     <tableColumn id="6" xr3:uid="{C68BBEAC-7A58-41FB-BA92-351982A4DA1B}" name="Folder Name" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Folder Id" totalsRowFunction="count" dataDxfId="3"/>
   </tableColumns>
@@ -596,7 +596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -606,7 +606,8 @@
     <col min="2" max="2" width="18.36328125" style="1" customWidth="1"/>
     <col min="3" max="3" width="48.81640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="47.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -620,16 +621,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -1181,7 +1182,8 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.36328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.36328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -1189,13 +1191,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -1629,7 +1631,8 @@
     <col min="2" max="2" width="18.36328125" style="1" customWidth="1"/>
     <col min="3" max="3" width="48.81640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="47.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -1643,16 +1646,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -2196,7 +2199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B90804-4CC2-4F3A-A5A0-B313E9BACDDF}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2222,16 +2225,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
GetFolders now return a dictionary of Dictionary(Of String, String) to avoid extra type conversions.
</commit_message>
<xml_diff>
--- a/Config/Assets.xlsx
+++ b/Config/Assets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B51AF56-9024-4A02-98CA-675E92F14E63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB05636-8BA3-4681-A917-AA1DCBFB9C6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -117,39 +117,6 @@
   </cellStyles>
   <dxfs count="15">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
@@ -257,6 +224,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -278,9 +278,9 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Value"/>
-    <tableColumn id="7" xr3:uid="{9F5282FE-6479-41B7-8672-34D0C5F6C8EE}" name="Folder Id or Path" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{42F54A22-BA7B-4DC3-BF4D-BA0546417160}" name="Asset Id" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{E2F843A0-E163-4591-A90A-DA03F637285C}" name="Result" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{9F5282FE-6479-41B7-8672-34D0C5F6C8EE}" name="Folder Id or Path" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{42F54A22-BA7B-4DC3-BF4D-BA0546417160}" name="Asset Id" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{E2F843A0-E163-4591-A90A-DA03F637285C}" name="Result" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -290,10 +290,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:D101" totalsRowShown="0">
   <autoFilter ref="A1:D101" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{51051268-0C6E-425F-8AEE-5BD7400426FE}" name="Folder Id or Path" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Asset Id" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{789EC9DB-B69B-4343-B58A-CF450EDB59BF}" name="Result" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{51051268-0C6E-425F-8AEE-5BD7400426FE}" name="Folder Id or Path" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Asset Id" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{789EC9DB-B69B-4343-B58A-CF450EDB59BF}" name="Result" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -307,9 +307,9 @@
     <tableColumn id="2" xr3:uid="{A5B9750D-9F4C-4ACD-B998-452D86A89786}" name="Type"/>
     <tableColumn id="3" xr3:uid="{C90CC352-910C-44A1-9626-F6DC71398CF0}" name="Description"/>
     <tableColumn id="4" xr3:uid="{FB9ABF1E-6D2B-4148-9C75-B26D470A604D}" name="Value"/>
-    <tableColumn id="7" xr3:uid="{D7BAAF9B-F2D3-47F6-A40B-80DD0288C534}" name="Folder Id or Path" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{C8CEBD6B-CDA3-4576-9A18-16C14163ADBC}" name="Asset Id" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{34576645-A498-4AA2-BA38-3776D490DE1A}" name="Result" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{D7BAAF9B-F2D3-47F6-A40B-80DD0288C534}" name="Folder Id or Path" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{C8CEBD6B-CDA3-4576-9A18-16C14163ADBC}" name="Asset Id" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{34576645-A498-4AA2-BA38-3776D490DE1A}" name="Result" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -321,11 +321,11 @@
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Type"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Description" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Value" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{A067D188-197D-4A79-82E6-8C9B8EDABB7C}" name="Asset Id" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{C68BBEAC-7A58-41FB-BA92-351982A4DA1B}" name="Folder Name" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Folder Id" totalsRowFunction="count" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Description" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Value" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{A067D188-197D-4A79-82E6-8C9B8EDABB7C}" name="Asset Id" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{C68BBEAC-7A58-41FB-BA92-351982A4DA1B}" name="Folder Name" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Folder Id" totalsRowFunction="count" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1155,12 +1155,9 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="2">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{F44B3D79-6E85-4752-80E5-E171C2D51A7E}">
       <formula1>"Text,Bool,Integer,Credential"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{0C12A5C3-BDEF-4B44-B330-2C8ED24D0DA9}">
-      <formula1>"Success,Failure"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed order or columns in sheets for better usability.
</commit_message>
<xml_diff>
--- a/Config/Assets.xlsx
+++ b/Config/Assets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B528F81E-1AEC-44B9-A120-A9B7684F1133}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CBFE2D-A688-4F28-A5BF-604711AAD709}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create" sheetId="1" r:id="rId1"/>
@@ -53,13 +53,13 @@
     <t>Result</t>
   </si>
   <si>
-    <t>Folder Name</t>
-  </si>
-  <si>
     <t>Asset Id</t>
   </si>
   <si>
     <t>Folder Id or Path</t>
+  </si>
+  <si>
+    <t>Folder Path</t>
   </si>
 </sst>
 </file>
@@ -314,9 +314,9 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Type"/>
     <tableColumn id="7" xr3:uid="{A067D188-197D-4A79-82E6-8C9B8EDABB7C}" name="Value" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{C68BBEAC-7A58-41FB-BA92-351982A4DA1B}" name="Asset Id" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Folder Name" totalsRowFunction="count" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{96DFDB45-0B9C-4367-9B24-D26DAD7C70E7}" name="Folder Id"/>
+    <tableColumn id="6" xr3:uid="{C68BBEAC-7A58-41FB-BA92-351982A4DA1B}" name="Folder Id" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Folder Path" totalsRowFunction="count" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{96DFDB45-0B9C-4367-9B24-D26DAD7C70E7}" name="Asset Id"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -587,7 +587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -597,7 +597,7 @@
     <col min="2" max="2" width="18.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="47.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -611,10 +611,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1246,8 +1246,8 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1255,10 +1255,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -1763,8 +1763,8 @@
     <col min="1" max="1" width="13" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="47.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.5703125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1779,10 +1779,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -2316,7 +2316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B90804-4CC2-4F3A-A5A0-B313E9BACDDF}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2324,7 +2324,7 @@
   <cols>
     <col min="1" max="1" width="13" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
@@ -2341,13 +2341,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>